<commit_message>
Add Section 04 BMS schematic with protection and balancing
BMS circuit features:
- HY2120-CB 2S protection IC (overcharge/overdischarge/overcurrent)
- HY2213-BB3A cell balancers (2x) with 62Ω bleed resistors
- AO3400A MOSFETs (4x) in back-to-back configuration
- 5mΩ current sense resistor (40A trip threshold)

Calculations added:
- Protection threshold analysis
- Current sense resistor sizing (200mV/40A = 5mΩ)
- Cell balancing resistor sizing (4.2V/68mA = 62Ω)
- MOSFET conduction loss analysis

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projects/IMSAFE_Assistant/IMSAFE/docs/07-calculations/IMSAFE_Schematic_Calculations.xlsx
+++ b/projects/IMSAFE_Assistant/IMSAFE/docs/07-calculations/IMSAFE_Schematic_Calculations.xlsx
@@ -11,7 +11,8 @@
     <sheet name="01_MCU_Core" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="02_USB_C" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="03_Charger" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Power_Budget" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="04_BMS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Power_Budget" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -480,7 +481,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Generated: 2026-01-28 20:29</t>
+          <t>Generated: 2026-01-28 20:39</t>
         </is>
       </c>
     </row>
@@ -614,17 +615,17 @@
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>Cell balancing calculations</t>
+          <t>Cell protection &amp; balancing</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Complete</t>
         </is>
       </c>
       <c r="D10" s="4" t="inlineStr">
         <is>
-          <t>~12</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -3456,6 +3457,1739 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F67"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Section 04: Battery Management System (BMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Battery Configuration</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Cell Configuration</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>2S</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>2 cells in series</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Cell Voltage (nom)</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Vcell</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>Li-ion nominal</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>Cell Voltage (max)</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Vcell_max</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>Full charge</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>Cell Voltage (min)</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Vcell_min</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>Discharge cutoff</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>Pack Voltage (nom)</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Vpack</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E9" s="4">
+        <f>2*3.7</f>
+        <v/>
+      </c>
+      <c r="F9" s="4" t="inlineStr">
+        <is>
+          <t>2S nominal</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>Pack Voltage (max)</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>Vpack_max</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E10" s="4">
+        <f>2*4.2</f>
+        <v/>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t>2S full charge</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>Pack Capacity</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>Cbat</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>mAh</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="inlineStr">
+        <is>
+          <t>Per spec</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>HY2120 Protection Thresholds</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Overcharge Threshold</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>Voc</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="D15" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>Per cell, CB version</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Overcharge Release</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>Vocr</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="D16" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" s="4" t="inlineStr">
+        <is>
+          <t>Hysteresis</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>Over-discharge Threshold</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>Vod</t>
+        </is>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>Per cell</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Over-discharge Release</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>Vodr</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>Hysteresis</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>Overcurrent (discharge)</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>Ioc_dis</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="D19" s="4" t="inlineStr">
+        <is>
+          <t>mV</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" s="4" t="inlineStr">
+        <is>
+          <t>Across sense resistor</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>Overcurrent (charge)</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>Ioc_chg</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>mV</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" s="4" t="inlineStr">
+        <is>
+          <t>Lower for charging</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Short Circuit</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>Isc</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>400</v>
+      </c>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>mV</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="inlineStr">
+        <is>
+          <t>Fast response</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Current Sense Resistor Calculation</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>Overcurrent Threshold</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>Voc</t>
+        </is>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="D25" s="4" t="inlineStr">
+        <is>
+          <t>mV</t>
+        </is>
+      </c>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>HY2120 typical</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>Desired Trip Current</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>Itrip</t>
+        </is>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="D26" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>Max continuous</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>Sense Resistor</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>R403</t>
+        </is>
+      </c>
+      <c r="C27" s="4">
+        <f>200/40</f>
+        <v/>
+      </c>
+      <c r="D27" s="4" t="inlineStr">
+        <is>
+          <t>mΩ</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>Rsense = Voc/Itrip</t>
+        </is>
+      </c>
+      <c r="F27" s="4" t="inlineStr">
+        <is>
+          <t>5mΩ calculated</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="inlineStr">
+        <is>
+          <t>Selected Value</t>
+        </is>
+      </c>
+      <c r="B28" s="4" t="inlineStr">
+        <is>
+          <t>R403</t>
+        </is>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4" t="inlineStr">
+        <is>
+          <t>mΩ</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" s="4" t="inlineStr">
+        <is>
+          <t>Standard 1% value</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="inlineStr">
+        <is>
+          <t>Actual Trip Current</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>Itrip_act</t>
+        </is>
+      </c>
+      <c r="C29" s="4">
+        <f>200/5</f>
+        <v/>
+      </c>
+      <c r="D29" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr">
+        <is>
+          <t>I = Voc/R</t>
+        </is>
+      </c>
+      <c r="F29" s="4" t="inlineStr">
+        <is>
+          <t>40A</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>Power @ Trip</t>
+        </is>
+      </c>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>Psense</t>
+        </is>
+      </c>
+      <c r="C30" s="4">
+        <f>40^2*5/1000</f>
+        <v/>
+      </c>
+      <c r="D30" s="4" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E30" s="4" t="inlineStr">
+        <is>
+          <t>P = I²R</t>
+        </is>
+      </c>
+      <c r="F30" s="4" t="inlineStr">
+        <is>
+          <t>8W peak</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="inlineStr">
+        <is>
+          <t>Power @ 5A Normal</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>Psense_5A</t>
+        </is>
+      </c>
+      <c r="C31" s="4">
+        <f>5^2*5/1000</f>
+        <v/>
+      </c>
+      <c r="D31" s="4" t="inlineStr">
+        <is>
+          <t>mW</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="inlineStr">
+        <is>
+          <t>P = I²R</t>
+        </is>
+      </c>
+      <c r="F31" s="4" t="inlineStr">
+        <is>
+          <t>125mW</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="inlineStr">
+        <is>
+          <t>Resistor Package</t>
+        </is>
+      </c>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>1206</t>
+        </is>
+      </c>
+      <c r="D32" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>0.5W rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Cell Balancing (HY2213-BB3A)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E35" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="inlineStr">
+        <is>
+          <t>Balance Start Voltage</t>
+        </is>
+      </c>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t>Vbal</t>
+        </is>
+      </c>
+      <c r="C36" s="4" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D36" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E36" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F36" s="4" t="inlineStr">
+        <is>
+          <t>HY2213-BB3A threshold</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="inlineStr">
+        <is>
+          <t>Balance Voltage Hyst</t>
+        </is>
+      </c>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>Vbal_h</t>
+        </is>
+      </c>
+      <c r="C37" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="D37" s="4" t="inlineStr">
+        <is>
+          <t>mV</t>
+        </is>
+      </c>
+      <c r="E37" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F37" s="4" t="inlineStr">
+        <is>
+          <t>Hysteresis</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="inlineStr">
+        <is>
+          <t>Desired Bleed Current</t>
+        </is>
+      </c>
+      <c r="B38" s="4" t="inlineStr">
+        <is>
+          <t>Ibal</t>
+        </is>
+      </c>
+      <c r="C38" s="4" t="n">
+        <v>68</v>
+      </c>
+      <c r="D38" s="4" t="inlineStr">
+        <is>
+          <t>mA</t>
+        </is>
+      </c>
+      <c r="E38" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F38" s="4" t="inlineStr">
+        <is>
+          <t>Moderate balance rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="inlineStr">
+        <is>
+          <t>Balance Resistor</t>
+        </is>
+      </c>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>Rbal</t>
+        </is>
+      </c>
+      <c r="C39" s="4">
+        <f>4.2/0.068</f>
+        <v/>
+      </c>
+      <c r="D39" s="4" t="inlineStr">
+        <is>
+          <t>Ω</t>
+        </is>
+      </c>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
+          <t>R = V/I</t>
+        </is>
+      </c>
+      <c r="F39" s="4" t="inlineStr">
+        <is>
+          <t>~62Ω</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="inlineStr">
+        <is>
+          <t>Selected Value</t>
+        </is>
+      </c>
+      <c r="B40" s="4" t="inlineStr">
+        <is>
+          <t>R404/R405</t>
+        </is>
+      </c>
+      <c r="C40" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="D40" s="4" t="inlineStr">
+        <is>
+          <t>Ω</t>
+        </is>
+      </c>
+      <c r="E40" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F40" s="4" t="inlineStr">
+        <is>
+          <t>Standard E24 value</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="inlineStr">
+        <is>
+          <t>Actual Bleed Current</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>Ibal_act</t>
+        </is>
+      </c>
+      <c r="C41" s="4">
+        <f>4.2/62*1000</f>
+        <v/>
+      </c>
+      <c r="D41" s="4" t="inlineStr">
+        <is>
+          <t>mA</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="inlineStr">
+        <is>
+          <t>I = V/R</t>
+        </is>
+      </c>
+      <c r="F41" s="4" t="inlineStr">
+        <is>
+          <t>67.7mA</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Power Dissipation</t>
+        </is>
+      </c>
+      <c r="B42" s="4" t="inlineStr">
+        <is>
+          <t>Pbal</t>
+        </is>
+      </c>
+      <c r="C42" s="4">
+        <f>4.2^2/62*1000</f>
+        <v/>
+      </c>
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>mW</t>
+        </is>
+      </c>
+      <c r="E42" s="4" t="inlineStr">
+        <is>
+          <t>P = V²/R</t>
+        </is>
+      </c>
+      <c r="F42" s="4" t="inlineStr">
+        <is>
+          <t>284mW</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>Resistor Package</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>0805</t>
+        </is>
+      </c>
+      <c r="D43" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E43" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F43" s="4" t="inlineStr">
+        <is>
+          <t>0.25W rating OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="inlineStr">
+        <is>
+          <t>Max Balance Time</t>
+        </is>
+      </c>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>t_bal</t>
+        </is>
+      </c>
+      <c r="C44" s="4">
+        <f>500/67.7</f>
+        <v/>
+      </c>
+      <c r="D44" s="4" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="E44" s="4" t="inlineStr">
+        <is>
+          <t>ΔQ / Ibal</t>
+        </is>
+      </c>
+      <c r="F44" s="4" t="inlineStr">
+        <is>
+          <t>~7.4h for 500mAh diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>MOSFET Selection (AO3400A)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="inlineStr">
+        <is>
+          <t>Drain-Source Voltage</t>
+        </is>
+      </c>
+      <c r="B48" s="4" t="inlineStr">
+        <is>
+          <t>Vds</t>
+        </is>
+      </c>
+      <c r="C48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D48" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E48" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F48" s="4" t="inlineStr">
+        <is>
+          <t>Exceeds 8.4V pack</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="inlineStr">
+        <is>
+          <t>Continuous Current</t>
+        </is>
+      </c>
+      <c r="B49" s="4" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="C49" s="4" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="D49" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E49" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F49" s="4" t="inlineStr">
+        <is>
+          <t>At 25°C</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="inlineStr">
+        <is>
+          <t>On Resistance</t>
+        </is>
+      </c>
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t>Rds_on</t>
+        </is>
+      </c>
+      <c r="C50" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="D50" s="4" t="inlineStr">
+        <is>
+          <t>mΩ</t>
+        </is>
+      </c>
+      <c r="E50" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F50" s="4" t="inlineStr">
+        <is>
+          <t>At Vgs=4.5V</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="inlineStr">
+        <is>
+          <t>Gate Threshold</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>Vgs_th</t>
+        </is>
+      </c>
+      <c r="C51" s="4" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="D51" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F51" s="4" t="inlineStr">
+        <is>
+          <t>Typical</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="inlineStr">
+        <is>
+          <t>HY2120 Gate Drive</t>
+        </is>
+      </c>
+      <c r="B52" s="4" t="inlineStr">
+        <is>
+          <t>Vgate</t>
+        </is>
+      </c>
+      <c r="C52" s="4" t="inlineStr">
+        <is>
+          <t>~3</t>
+        </is>
+      </c>
+      <c r="D52" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E52" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>From OD/OC pins</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="inlineStr">
+        <is>
+          <t>FETs in Series</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="C53" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D53" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E53" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F53" s="4" t="inlineStr">
+        <is>
+          <t>Back-to-back per function</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="inlineStr">
+        <is>
+          <t>Total Rds (per path)</t>
+        </is>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>Rds_total</t>
+        </is>
+      </c>
+      <c r="C54" s="4">
+        <f>28*2</f>
+        <v/>
+      </c>
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>mΩ</t>
+        </is>
+      </c>
+      <c r="E54" s="4" t="inlineStr">
+        <is>
+          <t>n * Rds_on</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>56mΩ</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="inlineStr">
+        <is>
+          <t>Conduction Loss @5A</t>
+        </is>
+      </c>
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t>Pcond</t>
+        </is>
+      </c>
+      <c r="C55" s="4">
+        <f>5^2*56/1000</f>
+        <v/>
+      </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>P = I² * R</t>
+        </is>
+      </c>
+      <c r="F55" s="4" t="inlineStr">
+        <is>
+          <t>1.4W</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="inlineStr">
+        <is>
+          <t>Gate Resistor</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>R401/R402</t>
+        </is>
+      </c>
+      <c r="C56" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4" t="inlineStr">
+        <is>
+          <t>kΩ</t>
+        </is>
+      </c>
+      <c r="E56" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>Limits gate current</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>Section 04 BOM Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="inlineStr">
+        <is>
+          <t>Reference</t>
+        </is>
+      </c>
+      <c r="B59" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C59" s="3" t="inlineStr">
+        <is>
+          <t>Package</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="E59" s="3" t="inlineStr">
+        <is>
+          <t>JLCPCB</t>
+        </is>
+      </c>
+      <c r="F59" s="3" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="4" t="inlineStr">
+        <is>
+          <t>U4</t>
+        </is>
+      </c>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>HY2120-CB</t>
+        </is>
+      </c>
+      <c r="C60" s="4" t="inlineStr">
+        <is>
+          <t>SOT-23-6</t>
+        </is>
+      </c>
+      <c r="D60" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4" t="inlineStr">
+        <is>
+          <t>C113632</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>2S protection IC</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="4" t="inlineStr">
+        <is>
+          <t>U5, U6</t>
+        </is>
+      </c>
+      <c r="B61" s="4" t="inlineStr">
+        <is>
+          <t>HY2213-BB3A</t>
+        </is>
+      </c>
+      <c r="C61" s="4" t="inlineStr">
+        <is>
+          <t>SOT-23-6</t>
+        </is>
+      </c>
+      <c r="D61" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" s="4" t="inlineStr">
+        <is>
+          <t>C113633</t>
+        </is>
+      </c>
+      <c r="F61" s="4" t="inlineStr">
+        <is>
+          <t>Cell balancer</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="4" t="inlineStr">
+        <is>
+          <t>Q1-Q4</t>
+        </is>
+      </c>
+      <c r="B62" s="4" t="inlineStr">
+        <is>
+          <t>AO3400A</t>
+        </is>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+      <c r="D62" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E62" s="4" t="inlineStr">
+        <is>
+          <t>C20917</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>N-ch MOSFET</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="4" t="inlineStr">
+        <is>
+          <t>C401-C403</t>
+        </is>
+      </c>
+      <c r="B63" s="4" t="inlineStr">
+        <is>
+          <t>100nF</t>
+        </is>
+      </c>
+      <c r="C63" s="4" t="inlineStr">
+        <is>
+          <t>0603</t>
+        </is>
+      </c>
+      <c r="D63" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E63" s="4" t="inlineStr">
+        <is>
+          <t>C14663</t>
+        </is>
+      </c>
+      <c r="F63" s="4" t="inlineStr">
+        <is>
+          <t>Bypass caps</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="inlineStr">
+        <is>
+          <t>R401, R402</t>
+        </is>
+      </c>
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t>1kΩ</t>
+        </is>
+      </c>
+      <c r="C64" s="4" t="inlineStr">
+        <is>
+          <t>0603</t>
+        </is>
+      </c>
+      <c r="D64" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E64" s="4" t="inlineStr">
+        <is>
+          <t>C21190</t>
+        </is>
+      </c>
+      <c r="F64" s="4" t="inlineStr">
+        <is>
+          <t>Gate resistors</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="inlineStr">
+        <is>
+          <t>R403</t>
+        </is>
+      </c>
+      <c r="B65" s="4" t="inlineStr">
+        <is>
+          <t>5mΩ</t>
+        </is>
+      </c>
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>1206</t>
+        </is>
+      </c>
+      <c r="D65" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="4" t="inlineStr">
+        <is>
+          <t>C2933641</t>
+        </is>
+      </c>
+      <c r="F65" s="4" t="inlineStr">
+        <is>
+          <t>Current sense</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="4" t="inlineStr">
+        <is>
+          <t>R404, R405</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>62Ω</t>
+        </is>
+      </c>
+      <c r="C66" s="4" t="inlineStr">
+        <is>
+          <t>0805</t>
+        </is>
+      </c>
+      <c r="D66" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E66" s="4" t="inlineStr">
+        <is>
+          <t>C17828</t>
+        </is>
+      </c>
+      <c r="F66" s="4" t="inlineStr">
+        <is>
+          <t>Balance resistors</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D67" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="E67" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F67" s="4" t="inlineStr">
+        <is>
+          <t>4 ICs + 11 passives</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Add design review checkpoint and update calculations workbook
- Add Appendix F: Design Review Checkpoint to design-rationale.md
- Update Known Issues table with ERC remediation status
- Fix R602 value in calculations (24.3k -> 19.1k) to match schematic
- Regenerate Excel workbook with corrected 5V regulator values

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projects/IMSAFE_Assistant/IMSAFE/docs/07-calculations/IMSAFE_Schematic_Calculations.xlsx
+++ b/projects/IMSAFE_Assistant/IMSAFE/docs/07-calculations/IMSAFE_Schematic_Calculations.xlsx
@@ -12,7 +12,8 @@
     <sheet name="02_USB_C" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="03_Charger" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="04_BMS" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Power_Budget" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="05_06_Regulators" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Power_Budget" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -481,7 +482,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Generated: 2026-01-28 20:39</t>
+          <t>Generated: 2026-01-29 09:44</t>
         </is>
       </c>
     </row>
@@ -625,7 +626,7 @@
       </c>
       <c r="D10" s="4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -637,22 +638,22 @@
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>05_Regulators</t>
+          <t>05_06_Regulators</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>3.3V/5V regulator calculations</t>
+          <t>3.3V/5V buck regulator sizing</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Complete</t>
         </is>
       </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>~14</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -5190,6 +5191,1483 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Sections 05-06: DC-DC Buck Regulators</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>System Parameters</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Input Voltage (nom)</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Vin</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>VSYS from 2S battery</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Input Voltage (min)</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Vin_min</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>Battery discharged</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>Input Voltage (max)</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Vin_max</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>Battery full</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>Switching Frequency</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Fsw</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>MHz</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>TPS6213x default</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Section 05: TPS62133 (3.3V Fixed)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Output Voltage</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>Vout</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Fixed output version</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="inlineStr">
+        <is>
+          <t>Max Output Current</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>Iout_max</t>
+        </is>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>Continuous</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>Typical Load Current</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>Iout_typ</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>MCU + sensors</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Inductor Value</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D15" s="4" t="inlineStr">
+        <is>
+          <t>µH</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
+          <t>TI recommended</t>
+        </is>
+      </c>
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>1-2.2µH range</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Inductor Saturation</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>Isat</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
+          <t>&gt;Iout_max</t>
+        </is>
+      </c>
+      <c r="F16" s="4" t="inlineStr">
+        <is>
+          <t>Must not saturate</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>Input Cap (bulk)</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>C501</t>
+        </is>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>µF</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>X7R ceramic</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Input Cap (HF)</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>C502</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>nF</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>High frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>Output Cap (bulk)</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>C503+C504</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>44</v>
+      </c>
+      <c r="D19" s="4" t="inlineStr">
+        <is>
+          <t>µF</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
+          <t>2×22µF</t>
+        </is>
+      </c>
+      <c r="F19" s="4" t="inlineStr">
+        <is>
+          <t>Low ESR X7R</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>Output Cap (HF)</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>C505</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>nF</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" s="4" t="inlineStr">
+        <is>
+          <t>High frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Efficiency (typ)</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>η</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>92</v>
+      </c>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>@7.4V,1A</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="inlineStr">
+        <is>
+          <t>From datasheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>Power Loss @0.5A</t>
+        </is>
+      </c>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>Ploss</t>
+        </is>
+      </c>
+      <c r="C22" s="4">
+        <f>0.5*3.3*(1-0.92)/0.92</f>
+        <v/>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
+          <t>Pout*(1-η)/η</t>
+        </is>
+      </c>
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>~143mW</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Section 06: TPS62130 (5V Adjustable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>Feedback Reference</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>Vfb</t>
+        </is>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D26" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>Internal reference</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>FB Top Resistor</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>R601</t>
+        </is>
+      </c>
+      <c r="C27" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D27" s="4" t="inlineStr">
+        <is>
+          <t>kΩ</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" s="4" t="inlineStr">
+        <is>
+          <t>VOUT to FB</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="inlineStr">
+        <is>
+          <t>FB Bottom Resistor</t>
+        </is>
+      </c>
+      <c r="B28" s="4" t="inlineStr">
+        <is>
+          <t>R602</t>
+        </is>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>19.1</v>
+      </c>
+      <c r="D28" s="4" t="inlineStr">
+        <is>
+          <t>kΩ</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="inlineStr">
+        <is>
+          <t>C25947</t>
+        </is>
+      </c>
+      <c r="F28" s="4" t="inlineStr">
+        <is>
+          <t>FB to GND</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="inlineStr">
+        <is>
+          <t>Output Voltage</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>Vout</t>
+        </is>
+      </c>
+      <c r="C29" s="4">
+        <f>0.8*(1+100/19.1)</f>
+        <v/>
+      </c>
+      <c r="D29" s="4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr">
+        <is>
+          <t>Vfb*(1+R601/R602)</t>
+        </is>
+      </c>
+      <c r="F29" s="4" t="inlineStr">
+        <is>
+          <t>~5.03V</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>Max Output Current</t>
+        </is>
+      </c>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>Iout_max</t>
+        </is>
+      </c>
+      <c r="C30" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D30" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E30" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F30" s="4" t="inlineStr">
+        <is>
+          <t>Continuous</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="inlineStr">
+        <is>
+          <t>Typical Load Current</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>Iout_typ</t>
+        </is>
+      </c>
+      <c r="C31" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" s="4" t="inlineStr">
+        <is>
+          <t>LEDs + display</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="inlineStr">
+        <is>
+          <t>Inductor Value</t>
+        </is>
+      </c>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t>L3</t>
+        </is>
+      </c>
+      <c r="C32" s="4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D32" s="4" t="inlineStr">
+        <is>
+          <t>µH</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="inlineStr">
+        <is>
+          <t>TI recommended</t>
+        </is>
+      </c>
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>1-2.2µH range</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="inlineStr">
+        <is>
+          <t>Inductor Saturation</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>Isat</t>
+        </is>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E33" s="4" t="inlineStr">
+        <is>
+          <t>&gt;Iout_max</t>
+        </is>
+      </c>
+      <c r="F33" s="4" t="inlineStr">
+        <is>
+          <t>Must not saturate</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>Efficiency (typ)</t>
+        </is>
+      </c>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t>η</t>
+        </is>
+      </c>
+      <c r="C34" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="D34" s="4" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="E34" s="4" t="inlineStr">
+        <is>
+          <t>@7.4V,1A</t>
+        </is>
+      </c>
+      <c r="F34" s="4" t="inlineStr">
+        <is>
+          <t>Estimated</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="inlineStr">
+        <is>
+          <t>Power Loss @1A</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>Ploss</t>
+        </is>
+      </c>
+      <c r="C35" s="4">
+        <f>1*5*(1-0.90)/0.90</f>
+        <v/>
+      </c>
+      <c r="D35" s="4" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="inlineStr">
+        <is>
+          <t>Pout*(1-η)/η</t>
+        </is>
+      </c>
+      <c r="F35" s="4" t="inlineStr">
+        <is>
+          <t>~556mW</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>Inductor Selection Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="F38" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="inlineStr">
+        <is>
+          <t>Min Inductance</t>
+        </is>
+      </c>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>Lmin</t>
+        </is>
+      </c>
+      <c r="C39" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4" t="inlineStr">
+        <is>
+          <t>µH</t>
+        </is>
+      </c>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
+          <t>TI app note</t>
+        </is>
+      </c>
+      <c r="F39" s="4" t="inlineStr">
+        <is>
+          <t>For 2.5MHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="inlineStr">
+        <is>
+          <t>Max Inductance</t>
+        </is>
+      </c>
+      <c r="B40" s="4" t="inlineStr">
+        <is>
+          <t>Lmax</t>
+        </is>
+      </c>
+      <c r="C40" s="4" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="D40" s="4" t="inlineStr">
+        <is>
+          <t>µH</t>
+        </is>
+      </c>
+      <c r="E40" s="4" t="inlineStr">
+        <is>
+          <t>TI app note</t>
+        </is>
+      </c>
+      <c r="F40" s="4" t="inlineStr">
+        <is>
+          <t>Higher = less ripple</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="inlineStr">
+        <is>
+          <t>Selected Value</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D41" s="4" t="inlineStr">
+        <is>
+          <t>µH</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F41" s="4" t="inlineStr">
+        <is>
+          <t>Good compromise</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Peak Current</t>
+        </is>
+      </c>
+      <c r="B42" s="4" t="inlineStr">
+        <is>
+          <t>Ipk</t>
+        </is>
+      </c>
+      <c r="C42" s="4">
+        <f>Iout+ΔI/2</f>
+        <v/>
+      </c>
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E42" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F42" s="4" t="inlineStr">
+        <is>
+          <t>Must be &lt; Isat</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>Ripple Current (est)</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>ΔI</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>~30%</t>
+        </is>
+      </c>
+      <c r="D43" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E43" s="4" t="inlineStr">
+        <is>
+          <t>of Iout</t>
+        </is>
+      </c>
+      <c r="F43" s="4" t="inlineStr">
+        <is>
+          <t>Typical design</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="inlineStr">
+        <is>
+          <t>DC Resistance</t>
+        </is>
+      </c>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>Rdc</t>
+        </is>
+      </c>
+      <c r="C44" s="4" t="inlineStr">
+        <is>
+          <t>&lt;30</t>
+        </is>
+      </c>
+      <c r="D44" s="4" t="inlineStr">
+        <is>
+          <t>mΩ</t>
+        </is>
+      </c>
+      <c r="E44" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F44" s="4" t="inlineStr">
+        <is>
+          <t>Lower = better efficiency</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="inlineStr">
+        <is>
+          <t>Package</t>
+        </is>
+      </c>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C45" s="4" t="inlineStr">
+        <is>
+          <t>4×4mm</t>
+        </is>
+      </c>
+      <c r="D45" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F45" s="4" t="inlineStr">
+        <is>
+          <t>Shielded ferrite</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>Sections 05-06 BOM Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>Reference</t>
+        </is>
+      </c>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>Package</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>JLCPCB</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="inlineStr">
+        <is>
+          <t>U7</t>
+        </is>
+      </c>
+      <c r="B49" s="4" t="inlineStr">
+        <is>
+          <t>TPS62133RGTR</t>
+        </is>
+      </c>
+      <c r="C49" s="4" t="inlineStr">
+        <is>
+          <t>QFN-16</t>
+        </is>
+      </c>
+      <c r="D49" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="4" t="inlineStr">
+        <is>
+          <t>C128072</t>
+        </is>
+      </c>
+      <c r="F49" s="4" t="inlineStr">
+        <is>
+          <t>3.3V buck</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="inlineStr">
+        <is>
+          <t>U8</t>
+        </is>
+      </c>
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t>TPS62130RGTR</t>
+        </is>
+      </c>
+      <c r="C50" s="4" t="inlineStr">
+        <is>
+          <t>QFN-16</t>
+        </is>
+      </c>
+      <c r="D50" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="inlineStr">
+        <is>
+          <t>C128068</t>
+        </is>
+      </c>
+      <c r="F50" s="4" t="inlineStr">
+        <is>
+          <t>5V buck</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="inlineStr">
+        <is>
+          <t>L2, L3</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>1.5µH 4A</t>
+        </is>
+      </c>
+      <c r="C51" s="4" t="inlineStr">
+        <is>
+          <t>4×4mm</t>
+        </is>
+      </c>
+      <c r="D51" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>C408335</t>
+        </is>
+      </c>
+      <c r="F51" s="4" t="inlineStr">
+        <is>
+          <t>Shielded inductor</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="inlineStr">
+        <is>
+          <t>C501, C601</t>
+        </is>
+      </c>
+      <c r="B52" s="4" t="inlineStr">
+        <is>
+          <t>10µF 16V</t>
+        </is>
+      </c>
+      <c r="C52" s="4" t="inlineStr">
+        <is>
+          <t>0805</t>
+        </is>
+      </c>
+      <c r="D52" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" s="4" t="inlineStr">
+        <is>
+          <t>C15850</t>
+        </is>
+      </c>
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>Input bulk</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="inlineStr">
+        <is>
+          <t>C502, C602, C505, C605</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="inlineStr">
+        <is>
+          <t>100nF</t>
+        </is>
+      </c>
+      <c r="C53" s="4" t="inlineStr">
+        <is>
+          <t>0603</t>
+        </is>
+      </c>
+      <c r="D53" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E53" s="4" t="inlineStr">
+        <is>
+          <t>C14663</t>
+        </is>
+      </c>
+      <c r="F53" s="4" t="inlineStr">
+        <is>
+          <t>HF filter</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="inlineStr">
+        <is>
+          <t>C503, C504, C603, C604</t>
+        </is>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>22µF 10V</t>
+        </is>
+      </c>
+      <c r="C54" s="4" t="inlineStr">
+        <is>
+          <t>0805</t>
+        </is>
+      </c>
+      <c r="D54" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E54" s="4" t="inlineStr">
+        <is>
+          <t>C45783</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>Output bulk</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="inlineStr">
+        <is>
+          <t>R501, R601, R603</t>
+        </is>
+      </c>
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t>100kΩ</t>
+        </is>
+      </c>
+      <c r="C55" s="4" t="inlineStr">
+        <is>
+          <t>0603</t>
+        </is>
+      </c>
+      <c r="D55" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>C25803</t>
+        </is>
+      </c>
+      <c r="F55" s="4" t="inlineStr">
+        <is>
+          <t>EN pull-up, FB top</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="inlineStr">
+        <is>
+          <t>R602</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>24.3kΩ</t>
+        </is>
+      </c>
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>0603</t>
+        </is>
+      </c>
+      <c r="D56" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="4" t="inlineStr">
+        <is>
+          <t>C25959</t>
+        </is>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>FB bottom</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B57" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C57" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D57" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="E57" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F57" s="4" t="inlineStr">
+        <is>
+          <t>2 ICs + 2 inductors + 14 passives</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>